<commit_message>
lt: kthu hộp đen_ sơ đồ chuyển trạng thái, so sánh cặp; bài tập về 2 kỹ thuật trên
</commit_message>
<xml_diff>
--- a/BT345_kỹ thuật test hộp đen (decision table, state transion diagram  ).xlsx
+++ b/BT345_kỹ thuật test hộp đen (decision table, state transion diagram  ).xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="decision table" sheetId="1" r:id="rId1"/>
+    <sheet name="state transition diagram" sheetId="2" r:id="rId2"/>
+    <sheet name="pairewise testing" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="174">
   <si>
     <t>I. bài tập decision table</t>
   </si>
@@ -464,12 +466,114 @@
   <si>
     <t>giảm 0%</t>
   </si>
+  <si>
+    <t>bài tập sơ đồ trạng thái</t>
+  </si>
+  <si>
+    <t>từ giỏ hàng rỗng, nhấn thêm sản phẩm</t>
+  </si>
+  <si>
+    <t>đến trạng thái màn hình chứa sp</t>
+  </si>
+  <si>
+    <t>từ giỏ hàng chứa sp, nhấn thêm sản phẩm</t>
+  </si>
+  <si>
+    <t>đến trạng thái màn hình chứa sp, tăng số lượng</t>
+  </si>
+  <si>
+    <t>từ giỏ hàng chứa sp, nhấn mua hàng</t>
+  </si>
+  <si>
+    <t>đến trạng thái màn hình tổng hợp sp</t>
+  </si>
+  <si>
+    <t>từ màn hình tổng hợp sp, nhấn ok</t>
+  </si>
+  <si>
+    <t>đến màn hình thanh toán</t>
+  </si>
+  <si>
+    <t>từ màn hình tổng hợp sp, nhấn not ok</t>
+  </si>
+  <si>
+    <t>đến màn hình chứa sp</t>
+  </si>
+  <si>
+    <t>từ giỏ hàng chứa sp, nhấn bỏ sản phẩm</t>
+  </si>
+  <si>
+    <t>đến trạng thái màn hình chứa sp, giảm số lượng</t>
+  </si>
+  <si>
+    <t>từ giỏ hàng chứa sp , nhấn bỏ sp (sp cuối)</t>
+  </si>
+  <si>
+    <t>đến trạng thái giỏ hàng rỗng</t>
+  </si>
+  <si>
+    <t>bài tập so sánh căp</t>
+  </si>
+  <si>
+    <t>xác định số lượng đầu vào</t>
+  </si>
+  <si>
+    <t>loại kh</t>
+  </si>
+  <si>
+    <t>hình thức pay</t>
+  </si>
+  <si>
+    <t>trình duyệt access</t>
+  </si>
+  <si>
+    <t>xác định số lượng số testcase thủ công</t>
+  </si>
+  <si>
+    <t>= 6*3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> individual</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> companies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the usa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> india</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> china</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> australia</t>
+  </si>
+  <si>
+    <t>visa</t>
+  </si>
+  <si>
+    <t>mastercard</t>
+  </si>
+  <si>
+    <t>paypal</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>safari</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,8 +594,22 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -508,6 +626,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BC2E6"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -663,7 +787,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -695,7 +819,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -707,14 +852,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -734,29 +882,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -773,6 +910,92 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>408838</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="5895238" cy="2000000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>46933</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>56714</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="762000"/>
+          <a:ext cx="5533333" cy="3485714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1040,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="K180" sqref="K180"/>
+    <sheetView topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,12 +1275,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -1065,33 +1288,33 @@
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
@@ -1162,11 +1385,11 @@
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
@@ -1237,11 +1460,11 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -1250,11 +1473,11 @@
       <c r="B18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
@@ -1263,18 +1486,18 @@
       <c r="B19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="20"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="28"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="23"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="31"/>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
@@ -1283,11 +1506,11 @@
       <c r="B21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18"/>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
@@ -1296,11 +1519,11 @@
       <c r="B22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="18"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
@@ -1308,24 +1531,24 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
@@ -1396,11 +1619,11 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
@@ -1471,79 +1694,79 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11" t="s">
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>1</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11" t="s">
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>2</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11" t="s">
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>3</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -1551,41 +1774,41 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="24" t="s">
+      <c r="B46" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="25"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
@@ -1733,11 +1956,11 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
@@ -1885,113 +2108,113 @@
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B64" s="13" t="s">
+      <c r="B64" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14" t="s">
+      <c r="C65" s="21"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
+      <c r="G65" s="21"/>
+      <c r="H65" s="21"/>
+      <c r="I65" s="21"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>1</v>
       </c>
-      <c r="B66" s="11" t="s">
+      <c r="B66" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11" t="s">
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-      <c r="I66" s="11"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>2</v>
       </c>
-      <c r="B67" s="11" t="s">
+      <c r="B67" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11" t="s">
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="11"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>3</v>
       </c>
-      <c r="B68" s="11" t="s">
+      <c r="B68" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="11" t="s">
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="11"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>4</v>
       </c>
-      <c r="B69" s="11" t="s">
+      <c r="B69" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11" t="s">
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="11"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>5</v>
       </c>
-      <c r="B70" s="11" t="s">
+      <c r="B70" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C70" s="11"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
-      <c r="F70" s="11" t="s">
+      <c r="C70" s="15"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="15"/>
+      <c r="F70" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="G70" s="11"/>
-      <c r="H70" s="11"/>
-      <c r="I70" s="11"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
@@ -1999,63 +2222,63 @@
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B73" s="12" t="s">
+      <c r="B73" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C73" s="12"/>
-      <c r="D73" s="12"/>
-      <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
-      <c r="G73" s="12"/>
-      <c r="H73" s="12"/>
-      <c r="I73" s="12"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="19"/>
+      <c r="H73" s="19"/>
+      <c r="I73" s="19"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B74" s="12"/>
-      <c r="C74" s="12"/>
-      <c r="D74" s="12"/>
-      <c r="E74" s="12"/>
-      <c r="F74" s="12"/>
-      <c r="G74" s="12"/>
-      <c r="H74" s="12"/>
-      <c r="I74" s="12"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="19"/>
+      <c r="I74" s="19"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B75" s="12"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12"/>
-      <c r="E75" s="12"/>
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="12"/>
-      <c r="I75" s="12"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="19"/>
+      <c r="H75" s="19"/>
+      <c r="I75" s="19"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
-      <c r="E76" s="12"/>
-      <c r="F76" s="12"/>
-      <c r="G76" s="12"/>
-      <c r="H76" s="12"/>
-      <c r="I76" s="12"/>
+      <c r="B76" s="19"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="19"/>
+      <c r="I76" s="19"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B77" s="12"/>
-      <c r="C77" s="12"/>
-      <c r="D77" s="12"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
-      <c r="H77" s="12"/>
-      <c r="I77" s="12"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="19"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="19"/>
+      <c r="G77" s="19"/>
+      <c r="H77" s="19"/>
+      <c r="I77" s="19"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B78" s="13" t="s">
+      <c r="B78" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C78" s="13"/>
-      <c r="D78" s="13"/>
+      <c r="C78" s="20"/>
+      <c r="D78" s="20"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
@@ -2203,11 +2426,11 @@
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B85" s="13" t="s">
+      <c r="B85" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C85" s="13"/>
-      <c r="D85" s="13"/>
+      <c r="C85" s="20"/>
+      <c r="D85" s="20"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
@@ -2355,96 +2578,96 @@
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B92" s="13" t="s">
+      <c r="B92" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C92" s="13"/>
-      <c r="D92" s="13"/>
+      <c r="C92" s="20"/>
+      <c r="D92" s="20"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B93" s="14" t="s">
+      <c r="B93" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C93" s="14"/>
-      <c r="D93" s="14"/>
-      <c r="E93" s="14"/>
-      <c r="F93" s="14" t="s">
+      <c r="C93" s="21"/>
+      <c r="D93" s="21"/>
+      <c r="E93" s="21"/>
+      <c r="F93" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G93" s="14"/>
-      <c r="H93" s="14"/>
-      <c r="I93" s="14"/>
+      <c r="G93" s="21"/>
+      <c r="H93" s="21"/>
+      <c r="I93" s="21"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>1</v>
       </c>
-      <c r="B94" s="11" t="s">
+      <c r="B94" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="11"/>
-      <c r="F94" s="11" t="s">
+      <c r="C94" s="15"/>
+      <c r="D94" s="15"/>
+      <c r="E94" s="15"/>
+      <c r="F94" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G94" s="11"/>
-      <c r="H94" s="11"/>
-      <c r="I94" s="11"/>
+      <c r="G94" s="15"/>
+      <c r="H94" s="15"/>
+      <c r="I94" s="15"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>2</v>
       </c>
-      <c r="B95" s="11" t="s">
+      <c r="B95" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11"/>
-      <c r="F95" s="11" t="s">
+      <c r="C95" s="15"/>
+      <c r="D95" s="15"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G95" s="11"/>
-      <c r="H95" s="11"/>
-      <c r="I95" s="11"/>
+      <c r="G95" s="15"/>
+      <c r="H95" s="15"/>
+      <c r="I95" s="15"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>3</v>
       </c>
-      <c r="B96" s="11" t="s">
+      <c r="B96" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C96" s="11"/>
-      <c r="D96" s="11"/>
-      <c r="E96" s="11"/>
-      <c r="F96" s="11" t="s">
+      <c r="C96" s="15"/>
+      <c r="D96" s="15"/>
+      <c r="E96" s="15"/>
+      <c r="F96" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="G96" s="11"/>
-      <c r="H96" s="11"/>
-      <c r="I96" s="11"/>
+      <c r="G96" s="15"/>
+      <c r="H96" s="15"/>
+      <c r="I96" s="15"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>4</v>
       </c>
-      <c r="B97" s="11" t="s">
+      <c r="B97" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C97" s="11"/>
-      <c r="D97" s="11"/>
-      <c r="E97" s="11"/>
-      <c r="F97" s="11" t="s">
+      <c r="C97" s="15"/>
+      <c r="D97" s="15"/>
+      <c r="E97" s="15"/>
+      <c r="F97" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="G97" s="11"/>
-      <c r="H97" s="11"/>
-      <c r="I97" s="11"/>
+      <c r="G97" s="15"/>
+      <c r="H97" s="15"/>
+      <c r="I97" s="15"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
@@ -2452,79 +2675,79 @@
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B100" s="12" t="s">
+      <c r="B100" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C100" s="12"/>
-      <c r="D100" s="12"/>
-      <c r="E100" s="12"/>
-      <c r="F100" s="12"/>
-      <c r="G100" s="12"/>
-      <c r="H100" s="12"/>
-      <c r="I100" s="12"/>
-      <c r="J100" s="12"/>
+      <c r="C100" s="19"/>
+      <c r="D100" s="19"/>
+      <c r="E100" s="19"/>
+      <c r="F100" s="19"/>
+      <c r="G100" s="19"/>
+      <c r="H100" s="19"/>
+      <c r="I100" s="19"/>
+      <c r="J100" s="19"/>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B101" s="12"/>
-      <c r="C101" s="12"/>
-      <c r="D101" s="12"/>
-      <c r="E101" s="12"/>
-      <c r="F101" s="12"/>
-      <c r="G101" s="12"/>
-      <c r="H101" s="12"/>
-      <c r="I101" s="12"/>
-      <c r="J101" s="12"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="19"/>
+      <c r="G101" s="19"/>
+      <c r="H101" s="19"/>
+      <c r="I101" s="19"/>
+      <c r="J101" s="19"/>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B102" s="12"/>
-      <c r="C102" s="12"/>
-      <c r="D102" s="12"/>
-      <c r="E102" s="12"/>
-      <c r="F102" s="12"/>
-      <c r="G102" s="12"/>
-      <c r="H102" s="12"/>
-      <c r="I102" s="12"/>
-      <c r="J102" s="12"/>
+      <c r="B102" s="19"/>
+      <c r="C102" s="19"/>
+      <c r="D102" s="19"/>
+      <c r="E102" s="19"/>
+      <c r="F102" s="19"/>
+      <c r="G102" s="19"/>
+      <c r="H102" s="19"/>
+      <c r="I102" s="19"/>
+      <c r="J102" s="19"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B103" s="12"/>
-      <c r="C103" s="12"/>
-      <c r="D103" s="12"/>
-      <c r="E103" s="12"/>
-      <c r="F103" s="12"/>
-      <c r="G103" s="12"/>
-      <c r="H103" s="12"/>
-      <c r="I103" s="12"/>
-      <c r="J103" s="12"/>
+      <c r="B103" s="19"/>
+      <c r="C103" s="19"/>
+      <c r="D103" s="19"/>
+      <c r="E103" s="19"/>
+      <c r="F103" s="19"/>
+      <c r="G103" s="19"/>
+      <c r="H103" s="19"/>
+      <c r="I103" s="19"/>
+      <c r="J103" s="19"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B104" s="12"/>
-      <c r="C104" s="12"/>
-      <c r="D104" s="12"/>
-      <c r="E104" s="12"/>
-      <c r="F104" s="12"/>
-      <c r="G104" s="12"/>
-      <c r="H104" s="12"/>
-      <c r="I104" s="12"/>
-      <c r="J104" s="12"/>
+      <c r="B104" s="19"/>
+      <c r="C104" s="19"/>
+      <c r="D104" s="19"/>
+      <c r="E104" s="19"/>
+      <c r="F104" s="19"/>
+      <c r="G104" s="19"/>
+      <c r="H104" s="19"/>
+      <c r="I104" s="19"/>
+      <c r="J104" s="19"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B105" s="12"/>
-      <c r="C105" s="12"/>
-      <c r="D105" s="12"/>
-      <c r="E105" s="12"/>
-      <c r="F105" s="12"/>
-      <c r="G105" s="12"/>
-      <c r="H105" s="12"/>
-      <c r="I105" s="12"/>
-      <c r="J105" s="12"/>
+      <c r="B105" s="19"/>
+      <c r="C105" s="19"/>
+      <c r="D105" s="19"/>
+      <c r="E105" s="19"/>
+      <c r="F105" s="19"/>
+      <c r="G105" s="19"/>
+      <c r="H105" s="19"/>
+      <c r="I105" s="19"/>
+      <c r="J105" s="19"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B106" s="13" t="s">
+      <c r="B106" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C106" s="13"/>
-      <c r="D106" s="13"/>
+      <c r="C106" s="20"/>
+      <c r="D106" s="20"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
@@ -2672,28 +2895,28 @@
       </c>
     </row>
     <row r="112" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="29"/>
-      <c r="C112" s="29"/>
-      <c r="D112" s="29"/>
-      <c r="E112" s="29"/>
-      <c r="F112" s="29"/>
-      <c r="G112" s="29"/>
-      <c r="H112" s="29"/>
-      <c r="I112" s="29"/>
-      <c r="J112" s="29"/>
+      <c r="B112" s="12"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="12"/>
+      <c r="E112" s="12"/>
+      <c r="F112" s="12"/>
+      <c r="G112" s="12"/>
+      <c r="H112" s="12"/>
+      <c r="I112" s="12"/>
+      <c r="J112" s="12"/>
     </row>
     <row r="113" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="13" t="s">
+      <c r="B113" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C113" s="13"/>
-      <c r="D113" s="13"/>
-      <c r="E113" s="29"/>
-      <c r="F113" s="29"/>
-      <c r="G113" s="29"/>
-      <c r="H113" s="29"/>
-      <c r="I113" s="29"/>
-      <c r="J113" s="29"/>
+      <c r="C113" s="20"/>
+      <c r="D113" s="20"/>
+      <c r="E113" s="12"/>
+      <c r="F113" s="12"/>
+      <c r="G113" s="12"/>
+      <c r="H113" s="12"/>
+      <c r="I113" s="12"/>
+      <c r="J113" s="12"/>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
@@ -2702,173 +2925,173 @@
     </row>
     <row r="115" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B116" s="13" t="s">
+      <c r="B116" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C116" s="13"/>
-      <c r="D116" s="13"/>
+      <c r="C116" s="20"/>
+      <c r="D116" s="20"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B117" s="14" t="s">
+      <c r="B117" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C117" s="14"/>
-      <c r="D117" s="14"/>
-      <c r="E117" s="14"/>
-      <c r="F117" s="25" t="s">
+      <c r="C117" s="21"/>
+      <c r="D117" s="21"/>
+      <c r="E117" s="21"/>
+      <c r="F117" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G117" s="26"/>
-      <c r="H117" s="26"/>
-      <c r="I117" s="26"/>
-      <c r="J117" s="27"/>
+      <c r="G117" s="23"/>
+      <c r="H117" s="23"/>
+      <c r="I117" s="23"/>
+      <c r="J117" s="24"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>1</v>
       </c>
-      <c r="B118" s="11" t="s">
+      <c r="B118" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C118" s="11"/>
-      <c r="D118" s="11"/>
-      <c r="E118" s="11"/>
-      <c r="F118" s="15" t="s">
+      <c r="C118" s="15"/>
+      <c r="D118" s="15"/>
+      <c r="E118" s="15"/>
+      <c r="F118" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="G118" s="16"/>
-      <c r="H118" s="16"/>
-      <c r="I118" s="16"/>
-      <c r="J118" s="17"/>
+      <c r="G118" s="17"/>
+      <c r="H118" s="17"/>
+      <c r="I118" s="17"/>
+      <c r="J118" s="18"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>2</v>
       </c>
-      <c r="B119" s="11" t="s">
+      <c r="B119" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C119" s="11"/>
-      <c r="D119" s="11"/>
-      <c r="E119" s="11"/>
-      <c r="F119" s="15" t="s">
+      <c r="C119" s="15"/>
+      <c r="D119" s="15"/>
+      <c r="E119" s="15"/>
+      <c r="F119" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="G119" s="16"/>
-      <c r="H119" s="16"/>
-      <c r="I119" s="16"/>
-      <c r="J119" s="17"/>
+      <c r="G119" s="17"/>
+      <c r="H119" s="17"/>
+      <c r="I119" s="17"/>
+      <c r="J119" s="18"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>3</v>
       </c>
-      <c r="B120" s="11" t="s">
+      <c r="B120" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="C120" s="11"/>
-      <c r="D120" s="11"/>
-      <c r="E120" s="11"/>
-      <c r="F120" s="15" t="s">
+      <c r="C120" s="15"/>
+      <c r="D120" s="15"/>
+      <c r="E120" s="15"/>
+      <c r="F120" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="G120" s="16"/>
-      <c r="H120" s="16"/>
-      <c r="I120" s="16"/>
-      <c r="J120" s="17"/>
+      <c r="G120" s="17"/>
+      <c r="H120" s="17"/>
+      <c r="I120" s="17"/>
+      <c r="J120" s="18"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>4</v>
       </c>
-      <c r="B121" s="11" t="s">
+      <c r="B121" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="C121" s="11"/>
-      <c r="D121" s="11"/>
-      <c r="E121" s="11"/>
-      <c r="F121" s="15" t="s">
+      <c r="C121" s="15"/>
+      <c r="D121" s="15"/>
+      <c r="E121" s="15"/>
+      <c r="F121" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="G121" s="16"/>
-      <c r="H121" s="16"/>
-      <c r="I121" s="16"/>
-      <c r="J121" s="17"/>
+      <c r="G121" s="17"/>
+      <c r="H121" s="17"/>
+      <c r="I121" s="17"/>
+      <c r="J121" s="18"/>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>5</v>
       </c>
-      <c r="B122" s="11" t="s">
+      <c r="B122" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="C122" s="11"/>
-      <c r="D122" s="11"/>
-      <c r="E122" s="11"/>
-      <c r="F122" s="15" t="s">
+      <c r="C122" s="15"/>
+      <c r="D122" s="15"/>
+      <c r="E122" s="15"/>
+      <c r="F122" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="G122" s="16"/>
-      <c r="H122" s="16"/>
-      <c r="I122" s="16"/>
-      <c r="J122" s="17"/>
+      <c r="G122" s="17"/>
+      <c r="H122" s="17"/>
+      <c r="I122" s="17"/>
+      <c r="J122" s="18"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>6</v>
       </c>
-      <c r="B123" s="11" t="s">
+      <c r="B123" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C123" s="11"/>
-      <c r="D123" s="11"/>
-      <c r="E123" s="11"/>
-      <c r="F123" s="15" t="s">
+      <c r="C123" s="15"/>
+      <c r="D123" s="15"/>
+      <c r="E123" s="15"/>
+      <c r="F123" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="G123" s="16"/>
-      <c r="H123" s="16"/>
-      <c r="I123" s="16"/>
-      <c r="J123" s="17"/>
+      <c r="G123" s="17"/>
+      <c r="H123" s="17"/>
+      <c r="I123" s="17"/>
+      <c r="J123" s="18"/>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>7</v>
       </c>
-      <c r="B124" s="11" t="s">
+      <c r="B124" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="C124" s="11"/>
-      <c r="D124" s="11"/>
-      <c r="E124" s="11"/>
-      <c r="F124" s="15" t="s">
+      <c r="C124" s="15"/>
+      <c r="D124" s="15"/>
+      <c r="E124" s="15"/>
+      <c r="F124" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="G124" s="16"/>
-      <c r="H124" s="16"/>
-      <c r="I124" s="16"/>
-      <c r="J124" s="17"/>
+      <c r="G124" s="17"/>
+      <c r="H124" s="17"/>
+      <c r="I124" s="17"/>
+      <c r="J124" s="18"/>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>8</v>
       </c>
-      <c r="B125" s="11" t="s">
+      <c r="B125" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C125" s="11"/>
-      <c r="D125" s="11"/>
-      <c r="E125" s="11"/>
-      <c r="F125" s="15" t="s">
+      <c r="C125" s="15"/>
+      <c r="D125" s="15"/>
+      <c r="E125" s="15"/>
+      <c r="F125" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="G125" s="16"/>
-      <c r="H125" s="16"/>
-      <c r="I125" s="16"/>
-      <c r="J125" s="17"/>
+      <c r="G125" s="17"/>
+      <c r="H125" s="17"/>
+      <c r="I125" s="17"/>
+      <c r="J125" s="18"/>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B127" s="2" t="s">
@@ -2876,90 +3099,90 @@
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B128" s="12" t="s">
+      <c r="B128" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C128" s="12"/>
-      <c r="D128" s="12"/>
-      <c r="E128" s="12"/>
-      <c r="F128" s="12"/>
-      <c r="G128" s="12"/>
-      <c r="H128" s="12"/>
-      <c r="I128" s="12"/>
-      <c r="J128" s="12"/>
+      <c r="C128" s="19"/>
+      <c r="D128" s="19"/>
+      <c r="E128" s="19"/>
+      <c r="F128" s="19"/>
+      <c r="G128" s="19"/>
+      <c r="H128" s="19"/>
+      <c r="I128" s="19"/>
+      <c r="J128" s="19"/>
     </row>
     <row r="129" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B129" s="12"/>
-      <c r="C129" s="12"/>
-      <c r="D129" s="12"/>
-      <c r="E129" s="12"/>
-      <c r="F129" s="12"/>
-      <c r="G129" s="12"/>
-      <c r="H129" s="12"/>
-      <c r="I129" s="12"/>
-      <c r="J129" s="12"/>
+      <c r="B129" s="19"/>
+      <c r="C129" s="19"/>
+      <c r="D129" s="19"/>
+      <c r="E129" s="19"/>
+      <c r="F129" s="19"/>
+      <c r="G129" s="19"/>
+      <c r="H129" s="19"/>
+      <c r="I129" s="19"/>
+      <c r="J129" s="19"/>
     </row>
     <row r="130" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B130" s="12"/>
-      <c r="C130" s="12"/>
-      <c r="D130" s="12"/>
-      <c r="E130" s="12"/>
-      <c r="F130" s="12"/>
-      <c r="G130" s="12"/>
-      <c r="H130" s="12"/>
-      <c r="I130" s="12"/>
-      <c r="J130" s="12"/>
+      <c r="B130" s="19"/>
+      <c r="C130" s="19"/>
+      <c r="D130" s="19"/>
+      <c r="E130" s="19"/>
+      <c r="F130" s="19"/>
+      <c r="G130" s="19"/>
+      <c r="H130" s="19"/>
+      <c r="I130" s="19"/>
+      <c r="J130" s="19"/>
     </row>
     <row r="131" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B131" s="12"/>
-      <c r="C131" s="12"/>
-      <c r="D131" s="12"/>
-      <c r="E131" s="12"/>
-      <c r="F131" s="12"/>
-      <c r="G131" s="12"/>
-      <c r="H131" s="12"/>
-      <c r="I131" s="12"/>
-      <c r="J131" s="12"/>
+      <c r="B131" s="19"/>
+      <c r="C131" s="19"/>
+      <c r="D131" s="19"/>
+      <c r="E131" s="19"/>
+      <c r="F131" s="19"/>
+      <c r="G131" s="19"/>
+      <c r="H131" s="19"/>
+      <c r="I131" s="19"/>
+      <c r="J131" s="19"/>
     </row>
     <row r="132" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B132" s="12"/>
-      <c r="C132" s="12"/>
-      <c r="D132" s="12"/>
-      <c r="E132" s="12"/>
-      <c r="F132" s="12"/>
-      <c r="G132" s="12"/>
-      <c r="H132" s="12"/>
-      <c r="I132" s="12"/>
-      <c r="J132" s="12"/>
+      <c r="B132" s="19"/>
+      <c r="C132" s="19"/>
+      <c r="D132" s="19"/>
+      <c r="E132" s="19"/>
+      <c r="F132" s="19"/>
+      <c r="G132" s="19"/>
+      <c r="H132" s="19"/>
+      <c r="I132" s="19"/>
+      <c r="J132" s="19"/>
     </row>
     <row r="133" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B133" s="12"/>
-      <c r="C133" s="12"/>
-      <c r="D133" s="12"/>
-      <c r="E133" s="12"/>
-      <c r="F133" s="12"/>
-      <c r="G133" s="12"/>
-      <c r="H133" s="12"/>
-      <c r="I133" s="12"/>
-      <c r="J133" s="12"/>
+      <c r="B133" s="19"/>
+      <c r="C133" s="19"/>
+      <c r="D133" s="19"/>
+      <c r="E133" s="19"/>
+      <c r="F133" s="19"/>
+      <c r="G133" s="19"/>
+      <c r="H133" s="19"/>
+      <c r="I133" s="19"/>
+      <c r="J133" s="19"/>
     </row>
     <row r="134" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B134" s="12"/>
-      <c r="C134" s="12"/>
-      <c r="D134" s="12"/>
-      <c r="E134" s="12"/>
-      <c r="F134" s="12"/>
-      <c r="G134" s="12"/>
-      <c r="H134" s="12"/>
-      <c r="I134" s="12"/>
-      <c r="J134" s="12"/>
+      <c r="B134" s="19"/>
+      <c r="C134" s="19"/>
+      <c r="D134" s="19"/>
+      <c r="E134" s="19"/>
+      <c r="F134" s="19"/>
+      <c r="G134" s="19"/>
+      <c r="H134" s="19"/>
+      <c r="I134" s="19"/>
+      <c r="J134" s="19"/>
     </row>
     <row r="136" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B136" s="13" t="s">
+      <c r="B136" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C136" s="13"/>
-      <c r="D136" s="13"/>
+      <c r="C136" s="20"/>
+      <c r="D136" s="20"/>
     </row>
     <row r="137" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B137" s="3" t="s">
@@ -2977,10 +3200,10 @@
       <c r="F137" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G137" s="28"/>
-      <c r="H137" s="28"/>
-      <c r="I137" s="28"/>
-      <c r="J137" s="28"/>
+      <c r="G137" s="11"/>
+      <c r="H137" s="11"/>
+      <c r="I137" s="11"/>
+      <c r="J137" s="11"/>
     </row>
     <row r="138" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B138" s="4" t="s">
@@ -2998,10 +3221,10 @@
       <c r="F138" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G138" s="29"/>
-      <c r="H138" s="29"/>
-      <c r="I138" s="29"/>
-      <c r="J138" s="29"/>
+      <c r="G138" s="12"/>
+      <c r="H138" s="12"/>
+      <c r="I138" s="12"/>
+      <c r="J138" s="12"/>
     </row>
     <row r="139" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B139" s="4" t="s">
@@ -3038,11 +3261,11 @@
       </c>
     </row>
     <row r="142" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B142" s="13" t="s">
+      <c r="B142" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C142" s="13"/>
-      <c r="D142" s="13"/>
+      <c r="C142" s="20"/>
+      <c r="D142" s="20"/>
     </row>
     <row r="143" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B143" s="1" t="s">
@@ -3050,101 +3273,101 @@
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B145" s="13" t="s">
+      <c r="B145" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C145" s="13"/>
-      <c r="D145" s="13"/>
+      <c r="C145" s="20"/>
+      <c r="D145" s="20"/>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B146" s="14" t="s">
+      <c r="B146" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C146" s="14"/>
-      <c r="D146" s="14"/>
-      <c r="E146" s="14"/>
-      <c r="F146" s="25" t="s">
+      <c r="C146" s="21"/>
+      <c r="D146" s="21"/>
+      <c r="E146" s="21"/>
+      <c r="F146" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G146" s="26"/>
-      <c r="H146" s="26"/>
-      <c r="I146" s="26"/>
-      <c r="J146" s="27"/>
+      <c r="G146" s="23"/>
+      <c r="H146" s="23"/>
+      <c r="I146" s="23"/>
+      <c r="J146" s="24"/>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>1</v>
       </c>
-      <c r="B147" s="11" t="s">
+      <c r="B147" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C147" s="11"/>
-      <c r="D147" s="11"/>
-      <c r="E147" s="11"/>
-      <c r="F147" s="15" t="s">
+      <c r="C147" s="15"/>
+      <c r="D147" s="15"/>
+      <c r="E147" s="15"/>
+      <c r="F147" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="G147" s="16"/>
-      <c r="H147" s="16"/>
-      <c r="I147" s="16"/>
-      <c r="J147" s="17"/>
+      <c r="G147" s="17"/>
+      <c r="H147" s="17"/>
+      <c r="I147" s="17"/>
+      <c r="J147" s="18"/>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <v>2</v>
       </c>
-      <c r="B148" s="11" t="s">
+      <c r="B148" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="C148" s="11"/>
-      <c r="D148" s="11"/>
-      <c r="E148" s="11"/>
-      <c r="F148" s="15" t="s">
+      <c r="C148" s="15"/>
+      <c r="D148" s="15"/>
+      <c r="E148" s="15"/>
+      <c r="F148" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="G148" s="16"/>
-      <c r="H148" s="16"/>
-      <c r="I148" s="16"/>
-      <c r="J148" s="17"/>
+      <c r="G148" s="17"/>
+      <c r="H148" s="17"/>
+      <c r="I148" s="17"/>
+      <c r="J148" s="18"/>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>3</v>
       </c>
-      <c r="B149" s="11" t="s">
+      <c r="B149" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="C149" s="11"/>
-      <c r="D149" s="11"/>
-      <c r="E149" s="11"/>
-      <c r="F149" s="15" t="s">
+      <c r="C149" s="15"/>
+      <c r="D149" s="15"/>
+      <c r="E149" s="15"/>
+      <c r="F149" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="G149" s="16"/>
-      <c r="H149" s="16"/>
-      <c r="I149" s="16"/>
-      <c r="J149" s="17"/>
+      <c r="G149" s="17"/>
+      <c r="H149" s="17"/>
+      <c r="I149" s="17"/>
+      <c r="J149" s="18"/>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <v>4</v>
       </c>
-      <c r="B150" s="11" t="s">
+      <c r="B150" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="C150" s="11"/>
-      <c r="D150" s="11"/>
-      <c r="E150" s="11"/>
-      <c r="F150" s="15" t="s">
+      <c r="C150" s="15"/>
+      <c r="D150" s="15"/>
+      <c r="E150" s="15"/>
+      <c r="F150" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="G150" s="16"/>
-      <c r="H150" s="16"/>
-      <c r="I150" s="16"/>
-      <c r="J150" s="17"/>
+      <c r="G150" s="17"/>
+      <c r="H150" s="17"/>
+      <c r="I150" s="17"/>
+      <c r="J150" s="18"/>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B152" s="2" t="s">
@@ -3152,90 +3375,90 @@
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B153" s="12" t="s">
+      <c r="B153" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="C153" s="12"/>
-      <c r="D153" s="12"/>
-      <c r="E153" s="12"/>
-      <c r="F153" s="12"/>
-      <c r="G153" s="12"/>
-      <c r="H153" s="12"/>
-      <c r="I153" s="12"/>
-      <c r="J153" s="12"/>
+      <c r="C153" s="19"/>
+      <c r="D153" s="19"/>
+      <c r="E153" s="19"/>
+      <c r="F153" s="19"/>
+      <c r="G153" s="19"/>
+      <c r="H153" s="19"/>
+      <c r="I153" s="19"/>
+      <c r="J153" s="19"/>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B154" s="12"/>
-      <c r="C154" s="12"/>
-      <c r="D154" s="12"/>
-      <c r="E154" s="12"/>
-      <c r="F154" s="12"/>
-      <c r="G154" s="12"/>
-      <c r="H154" s="12"/>
-      <c r="I154" s="12"/>
-      <c r="J154" s="12"/>
+      <c r="B154" s="19"/>
+      <c r="C154" s="19"/>
+      <c r="D154" s="19"/>
+      <c r="E154" s="19"/>
+      <c r="F154" s="19"/>
+      <c r="G154" s="19"/>
+      <c r="H154" s="19"/>
+      <c r="I154" s="19"/>
+      <c r="J154" s="19"/>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B155" s="12"/>
-      <c r="C155" s="12"/>
-      <c r="D155" s="12"/>
-      <c r="E155" s="12"/>
-      <c r="F155" s="12"/>
-      <c r="G155" s="12"/>
-      <c r="H155" s="12"/>
-      <c r="I155" s="12"/>
-      <c r="J155" s="12"/>
+      <c r="B155" s="19"/>
+      <c r="C155" s="19"/>
+      <c r="D155" s="19"/>
+      <c r="E155" s="19"/>
+      <c r="F155" s="19"/>
+      <c r="G155" s="19"/>
+      <c r="H155" s="19"/>
+      <c r="I155" s="19"/>
+      <c r="J155" s="19"/>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B156" s="12"/>
-      <c r="C156" s="12"/>
-      <c r="D156" s="12"/>
-      <c r="E156" s="12"/>
-      <c r="F156" s="12"/>
-      <c r="G156" s="12"/>
-      <c r="H156" s="12"/>
-      <c r="I156" s="12"/>
-      <c r="J156" s="12"/>
+      <c r="B156" s="19"/>
+      <c r="C156" s="19"/>
+      <c r="D156" s="19"/>
+      <c r="E156" s="19"/>
+      <c r="F156" s="19"/>
+      <c r="G156" s="19"/>
+      <c r="H156" s="19"/>
+      <c r="I156" s="19"/>
+      <c r="J156" s="19"/>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B157" s="12"/>
-      <c r="C157" s="12"/>
-      <c r="D157" s="12"/>
-      <c r="E157" s="12"/>
-      <c r="F157" s="12"/>
-      <c r="G157" s="12"/>
-      <c r="H157" s="12"/>
-      <c r="I157" s="12"/>
-      <c r="J157" s="12"/>
+      <c r="B157" s="19"/>
+      <c r="C157" s="19"/>
+      <c r="D157" s="19"/>
+      <c r="E157" s="19"/>
+      <c r="F157" s="19"/>
+      <c r="G157" s="19"/>
+      <c r="H157" s="19"/>
+      <c r="I157" s="19"/>
+      <c r="J157" s="19"/>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B158" s="12"/>
-      <c r="C158" s="12"/>
-      <c r="D158" s="12"/>
-      <c r="E158" s="12"/>
-      <c r="F158" s="12"/>
-      <c r="G158" s="12"/>
-      <c r="H158" s="12"/>
-      <c r="I158" s="12"/>
-      <c r="J158" s="12"/>
+      <c r="B158" s="19"/>
+      <c r="C158" s="19"/>
+      <c r="D158" s="19"/>
+      <c r="E158" s="19"/>
+      <c r="F158" s="19"/>
+      <c r="G158" s="19"/>
+      <c r="H158" s="19"/>
+      <c r="I158" s="19"/>
+      <c r="J158" s="19"/>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B159" s="12"/>
-      <c r="C159" s="12"/>
-      <c r="D159" s="12"/>
-      <c r="E159" s="12"/>
-      <c r="F159" s="12"/>
-      <c r="G159" s="12"/>
-      <c r="H159" s="12"/>
-      <c r="I159" s="12"/>
-      <c r="J159" s="12"/>
+      <c r="B159" s="19"/>
+      <c r="C159" s="19"/>
+      <c r="D159" s="19"/>
+      <c r="E159" s="19"/>
+      <c r="F159" s="19"/>
+      <c r="G159" s="19"/>
+      <c r="H159" s="19"/>
+      <c r="I159" s="19"/>
+      <c r="J159" s="19"/>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B160" s="13" t="s">
+      <c r="B160" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C160" s="13"/>
-      <c r="D160" s="13"/>
+      <c r="C160" s="20"/>
+      <c r="D160" s="20"/>
       <c r="E160" s="10"/>
       <c r="F160" s="10"/>
     </row>
@@ -3359,25 +3582,25 @@
       <c r="B165" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C165" s="30">
+      <c r="C165" s="13">
         <v>0.2</v>
       </c>
       <c r="D165" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E165" s="31">
+      <c r="E165" s="14">
         <v>0.2</v>
       </c>
-      <c r="F165" s="30">
+      <c r="F165" s="13">
         <v>0.15</v>
       </c>
-      <c r="G165" s="30">
+      <c r="G165" s="13">
         <v>0.2</v>
       </c>
-      <c r="H165" s="30">
+      <c r="H165" s="13">
         <v>0.1</v>
       </c>
-      <c r="I165" s="30">
+      <c r="I165" s="13">
         <v>0.2</v>
       </c>
       <c r="J165" s="4">
@@ -3385,11 +3608,11 @@
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B167" s="13" t="s">
+      <c r="B167" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C167" s="13"/>
-      <c r="D167" s="13"/>
+      <c r="C167" s="20"/>
+      <c r="D167" s="20"/>
       <c r="E167" s="10"/>
       <c r="F167" s="10"/>
       <c r="G167" s="10"/>
@@ -3517,25 +3740,25 @@
       <c r="B172" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C172" s="30">
+      <c r="C172" s="13">
         <v>0.2</v>
       </c>
       <c r="D172" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E172" s="31">
+      <c r="E172" s="14">
         <v>0.2</v>
       </c>
-      <c r="F172" s="30">
+      <c r="F172" s="13">
         <v>0.15</v>
       </c>
-      <c r="G172" s="30">
+      <c r="G172" s="13">
         <v>0.2</v>
       </c>
-      <c r="H172" s="30">
+      <c r="H172" s="13">
         <v>0.1</v>
       </c>
-      <c r="I172" s="30">
+      <c r="I172" s="13">
         <v>0.2</v>
       </c>
       <c r="J172" s="4">
@@ -3544,11 +3767,11 @@
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="10"/>
-      <c r="B174" s="13" t="s">
+      <c r="B174" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C174" s="13"/>
-      <c r="D174" s="13"/>
+      <c r="C174" s="20"/>
+      <c r="D174" s="20"/>
       <c r="E174" s="10"/>
       <c r="F174" s="10"/>
       <c r="G174" s="10"/>
@@ -3560,133 +3783,170 @@
       <c r="A175" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B175" s="14" t="s">
+      <c r="B175" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C175" s="14"/>
-      <c r="D175" s="14"/>
-      <c r="E175" s="14"/>
-      <c r="F175" s="25" t="s">
+      <c r="C175" s="21"/>
+      <c r="D175" s="21"/>
+      <c r="E175" s="21"/>
+      <c r="F175" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G175" s="26"/>
-      <c r="H175" s="26"/>
-      <c r="I175" s="26"/>
-      <c r="J175" s="27"/>
+      <c r="G175" s="23"/>
+      <c r="H175" s="23"/>
+      <c r="I175" s="23"/>
+      <c r="J175" s="24"/>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="4">
         <v>1</v>
       </c>
-      <c r="B176" s="11" t="s">
+      <c r="B176" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="C176" s="11"/>
-      <c r="D176" s="11"/>
-      <c r="E176" s="11"/>
-      <c r="F176" s="15" t="s">
+      <c r="C176" s="15"/>
+      <c r="D176" s="15"/>
+      <c r="E176" s="15"/>
+      <c r="F176" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="G176" s="16"/>
-      <c r="H176" s="16"/>
-      <c r="I176" s="16"/>
-      <c r="J176" s="17"/>
+      <c r="G176" s="17"/>
+      <c r="H176" s="17"/>
+      <c r="I176" s="17"/>
+      <c r="J176" s="18"/>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="4">
         <v>2</v>
       </c>
-      <c r="B177" s="11" t="s">
+      <c r="B177" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C177" s="11"/>
-      <c r="D177" s="11"/>
-      <c r="E177" s="11"/>
-      <c r="F177" s="15" t="s">
+      <c r="C177" s="15"/>
+      <c r="D177" s="15"/>
+      <c r="E177" s="15"/>
+      <c r="F177" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G177" s="16"/>
-      <c r="H177" s="16"/>
-      <c r="I177" s="16"/>
-      <c r="J177" s="17"/>
+      <c r="G177" s="17"/>
+      <c r="H177" s="17"/>
+      <c r="I177" s="17"/>
+      <c r="J177" s="18"/>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="4">
         <v>3</v>
       </c>
-      <c r="B178" s="11" t="s">
+      <c r="B178" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="C178" s="11"/>
-      <c r="D178" s="11"/>
-      <c r="E178" s="11"/>
-      <c r="F178" s="15" t="s">
+      <c r="C178" s="15"/>
+      <c r="D178" s="15"/>
+      <c r="E178" s="15"/>
+      <c r="F178" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="G178" s="16"/>
-      <c r="H178" s="16"/>
-      <c r="I178" s="16"/>
-      <c r="J178" s="17"/>
+      <c r="G178" s="17"/>
+      <c r="H178" s="17"/>
+      <c r="I178" s="17"/>
+      <c r="J178" s="18"/>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="4">
         <v>4</v>
       </c>
-      <c r="B179" s="11" t="s">
+      <c r="B179" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="C179" s="11"/>
-      <c r="D179" s="11"/>
-      <c r="E179" s="11"/>
-      <c r="F179" s="15" t="s">
+      <c r="C179" s="15"/>
+      <c r="D179" s="15"/>
+      <c r="E179" s="15"/>
+      <c r="F179" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="G179" s="16"/>
-      <c r="H179" s="16"/>
-      <c r="I179" s="16"/>
-      <c r="J179" s="17"/>
+      <c r="G179" s="17"/>
+      <c r="H179" s="17"/>
+      <c r="I179" s="17"/>
+      <c r="J179" s="18"/>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="4">
         <v>5</v>
       </c>
-      <c r="B180" s="11" t="s">
+      <c r="B180" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="C180" s="11"/>
-      <c r="D180" s="11"/>
-      <c r="E180" s="11"/>
-      <c r="F180" s="15" t="s">
+      <c r="C180" s="15"/>
+      <c r="D180" s="15"/>
+      <c r="E180" s="15"/>
+      <c r="F180" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="G180" s="16"/>
-      <c r="H180" s="16"/>
-      <c r="I180" s="16"/>
-      <c r="J180" s="17"/>
+      <c r="G180" s="17"/>
+      <c r="H180" s="17"/>
+      <c r="I180" s="17"/>
+      <c r="J180" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="103">
-    <mergeCell ref="B179:E179"/>
-    <mergeCell ref="F179:J179"/>
-    <mergeCell ref="B180:E180"/>
-    <mergeCell ref="F180:J180"/>
-    <mergeCell ref="B176:E176"/>
-    <mergeCell ref="F176:J176"/>
-    <mergeCell ref="B177:E177"/>
-    <mergeCell ref="F177:J177"/>
-    <mergeCell ref="B178:E178"/>
-    <mergeCell ref="F178:J178"/>
-    <mergeCell ref="B153:J159"/>
-    <mergeCell ref="B160:D160"/>
-    <mergeCell ref="B167:D167"/>
-    <mergeCell ref="B174:D174"/>
-    <mergeCell ref="B175:E175"/>
-    <mergeCell ref="F175:J175"/>
-    <mergeCell ref="B149:E149"/>
-    <mergeCell ref="B150:E150"/>
-    <mergeCell ref="F148:J148"/>
-    <mergeCell ref="F149:J149"/>
-    <mergeCell ref="F150:J150"/>
+    <mergeCell ref="F95:I95"/>
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B3:I4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B73:I77"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="B92:D92"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="B46:F49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="F117:J117"/>
+    <mergeCell ref="F118:J118"/>
+    <mergeCell ref="B119:E119"/>
+    <mergeCell ref="B100:J105"/>
+    <mergeCell ref="B106:D106"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="B117:E117"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F69:I69"/>
+    <mergeCell ref="F70:I70"/>
+    <mergeCell ref="B93:E93"/>
+    <mergeCell ref="F93:I93"/>
+    <mergeCell ref="B94:E94"/>
+    <mergeCell ref="F94:I94"/>
+    <mergeCell ref="B95:E95"/>
+    <mergeCell ref="B96:E96"/>
+    <mergeCell ref="B97:E97"/>
     <mergeCell ref="B146:E146"/>
     <mergeCell ref="F146:J146"/>
     <mergeCell ref="B147:E147"/>
@@ -3711,66 +3971,693 @@
     <mergeCell ref="B123:E123"/>
     <mergeCell ref="B124:E124"/>
     <mergeCell ref="B118:E118"/>
-    <mergeCell ref="F117:J117"/>
-    <mergeCell ref="F118:J118"/>
-    <mergeCell ref="B119:E119"/>
-    <mergeCell ref="B100:J105"/>
-    <mergeCell ref="B106:D106"/>
-    <mergeCell ref="B116:D116"/>
-    <mergeCell ref="B117:E117"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F69:I69"/>
-    <mergeCell ref="F70:I70"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="B46:F49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B3:I4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B73:I77"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="B92:D92"/>
-    <mergeCell ref="B93:E93"/>
-    <mergeCell ref="F93:I93"/>
-    <mergeCell ref="B94:E94"/>
-    <mergeCell ref="F94:I94"/>
-    <mergeCell ref="B95:E95"/>
-    <mergeCell ref="B96:E96"/>
-    <mergeCell ref="B97:E97"/>
-    <mergeCell ref="F95:I95"/>
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="B153:J159"/>
+    <mergeCell ref="B160:D160"/>
+    <mergeCell ref="B167:D167"/>
+    <mergeCell ref="B174:D174"/>
+    <mergeCell ref="B175:E175"/>
+    <mergeCell ref="F175:J175"/>
+    <mergeCell ref="B149:E149"/>
+    <mergeCell ref="B150:E150"/>
+    <mergeCell ref="F148:J148"/>
+    <mergeCell ref="F149:J149"/>
+    <mergeCell ref="F150:J150"/>
+    <mergeCell ref="B179:E179"/>
+    <mergeCell ref="F179:J179"/>
+    <mergeCell ref="B180:E180"/>
+    <mergeCell ref="F180:J180"/>
+    <mergeCell ref="B176:E176"/>
+    <mergeCell ref="F176:J176"/>
+    <mergeCell ref="B177:E177"/>
+    <mergeCell ref="F177:J177"/>
+    <mergeCell ref="B178:E178"/>
+    <mergeCell ref="F178:J178"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:K23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
+        <v>1</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="18"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>2</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="18"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
+        <v>3</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="18"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="4">
+        <v>4</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="18"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
+        <v>5</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="18"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>6</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="18"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <v>7</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G17:K17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+    </row>
+    <row r="23" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="H24" s="36"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="34">
+        <v>6</v>
+      </c>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34">
+        <v>3</v>
+      </c>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34">
+        <v>3</v>
+      </c>
+      <c r="H25" s="34"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C31" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="H31" s="36"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="H32" s="34"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="H33" s="34"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="H34" s="34"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="H35" s="34"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="H36" s="34"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>6</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="F37" s="34"/>
+      <c r="G37" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="H37" s="34"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>7</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="H38" s="34"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>8</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="H39" s="34"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>9</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="H40" s="34"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>10</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="H41" s="34"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>11</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="H42" s="34"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>12</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="F43" s="34"/>
+      <c r="G43" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="H43" s="34"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>13</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="F44" s="34"/>
+      <c r="G44" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="H44" s="34"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>14</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="F45" s="34"/>
+      <c r="G45" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="H45" s="34"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>15</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="F46" s="34"/>
+      <c r="G46" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="H46" s="34"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>16</v>
+      </c>
+      <c r="C47" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="F47" s="34"/>
+      <c r="G47" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="H47" s="34"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>17</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="F48" s="34"/>
+      <c r="G48" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="H48" s="34"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>18</v>
+      </c>
+      <c r="C49" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="D49" s="34"/>
+      <c r="E49" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="H49" s="34"/>
+    </row>
+  </sheetData>
+  <mergeCells count="67">
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>